<commit_message>
A few more config files
</commit_message>
<xml_diff>
--- a/scenarios/01_original_data/cargo_train_schedule.xlsx
+++ b/scenarios/01_original_data/cargo_train_schedule.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\devsbb\eclipse-workspace\ibg\scenarios\01_original_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdealmeida\Documents\SBB Funding Proposal\Rail Supply\r009. medium scenario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C4377F-00BA-478B-A632-833A1D8278A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="936" yWindow="936" windowWidth="21600" windowHeight="12672" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="930" windowWidth="21600" windowHeight="12675"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="7" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$2:$K$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$2:$N$21</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="22">
   <si>
     <t>Zug</t>
   </si>
@@ -88,12 +87,6 @@
     <t>Gaeu</t>
   </si>
   <si>
-    <t>GE-GAEU-DT-GSS</t>
-  </si>
-  <si>
-    <t>GSS-DT-GAEU-GE</t>
-  </si>
-  <si>
     <t>Sottoceneri</t>
   </si>
   <si>
@@ -102,11 +95,32 @@
   <si>
     <t>DT-SC</t>
   </si>
+  <si>
+    <t>Basel</t>
+  </si>
+  <si>
+    <t>Lausanne</t>
+  </si>
+  <si>
+    <t>GE-LAUS-GAEU-DT-GSS</t>
+  </si>
+  <si>
+    <t>GSS-DT-GAEU-LAUS-GE</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>GAEU-BAS</t>
+  </si>
+  <si>
+    <t>BAS-GAEU</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -191,7 +205,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -324,11 +338,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -378,9 +403,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -664,19 +699,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED1ADEFE-053F-4679-8CCF-7AB2E47C65CE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N1048544"/>
+  <dimension ref="A1:T1048567"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E5" sqref="E5"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
@@ -684,15 +719,21 @@
     <col min="5" max="5" width="8.7109375" style="28"/>
     <col min="6" max="6" width="7.7109375" style="25" customWidth="1"/>
     <col min="7" max="7" width="7.7109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="7.7109375" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" style="27"/>
-    <col min="12" max="12" width="5.7109375" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" style="27" customWidth="1"/>
-    <col min="14" max="14" width="4.85546875" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="28"/>
+    <col min="9" max="9" width="7.7109375" style="25" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="7.7109375" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" style="27"/>
+    <col min="15" max="15" width="5.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" style="27" customWidth="1"/>
+    <col min="17" max="17" width="8.7109375" style="25"/>
+    <col min="18" max="18" width="5.7109375" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" style="27" customWidth="1"/>
+    <col min="20" max="20" width="4.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -705,26 +746,36 @@
       <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="42"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="40" t="s">
+      <c r="I1" s="38"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="24"/>
-      <c r="M1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="24"/>
-    </row>
-    <row r="2" spans="1:14" s="36" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O1" s="24"/>
+      <c r="P1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="T1" s="24"/>
+    </row>
+    <row r="2" spans="1:20" s="36" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
         <v>5</v>
       </c>
@@ -742,28 +793,41 @@
       <c r="G2" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="31" t="s">
         <v>6</v>
       </c>
       <c r="I2" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="L2" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="32" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N2" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="32"/>
+      <c r="S2" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C3" s="22">
         <v>1</v>
@@ -772,38 +836,51 @@
         <v>0.375</v>
       </c>
       <c r="E3" s="16">
-        <v>0.52083333333333337</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="F3" s="11">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="G3" s="10">
         <f>E3+F3</f>
+        <v>0.4375</v>
+      </c>
+      <c r="H3" s="16">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="I3" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="J3" s="10">
+        <f>H3+I3</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="H3" s="13">
+      <c r="K3" s="13">
         <v>0.57291666666666663</v>
       </c>
-      <c r="I3" s="11">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="J3" s="9">
-        <f>H3+I3</f>
+      <c r="L3" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="M3" s="9">
+        <f>K3+L3</f>
         <v>0.59375</v>
       </c>
-      <c r="K3" s="26">
+      <c r="N3" s="26">
         <v>0.64583333333333337</v>
       </c>
-      <c r="L3" s="19"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="19"/>
-    </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O3" s="19"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="30"/>
+      <c r="T3" s="19"/>
+    </row>
+    <row r="4" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C4" s="22">
         <v>2</v>
@@ -813,132 +890,1463 @@
       </c>
       <c r="E4" s="15">
         <f>G4+F4</f>
+        <v>0.59375</v>
+      </c>
+      <c r="F4" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G4" s="14">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="H4" s="15">
+        <f>J4+I4</f>
         <v>0.48958333333333331</v>
       </c>
-      <c r="F4" s="11">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="G4" s="14">
+      <c r="I4" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="J4" s="14">
         <v>0.46875</v>
       </c>
-      <c r="H4" s="9">
-        <f>J4+I4</f>
+      <c r="K4" s="9">
+        <f>M4+L4</f>
         <v>0.4375</v>
       </c>
-      <c r="I4" s="11">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="J4" s="13">
+      <c r="L4" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="M4" s="13">
         <v>0.41666666666666669</v>
       </c>
-      <c r="K4" s="12">
+      <c r="N4" s="12">
         <v>0.36458333333333331</v>
       </c>
-      <c r="L4" s="19"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="19"/>
-    </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="19"/>
-    </row>
-    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O4" s="19"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="19"/>
+    </row>
+    <row r="5" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="22">
+        <v>1</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E5" s="16">
+        <f>D5+(E3-D3)</f>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="F5" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G5" s="10">
+        <f>E5+F5</f>
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="H5" s="16">
+        <f>G5+(H3-G3)</f>
+        <v>0.6875</v>
+      </c>
+      <c r="I5" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="J5" s="10">
+        <f>H5+I5</f>
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="K5" s="16">
+        <f>J5+(K3-J3)</f>
+        <v>0.73958333333333326</v>
+      </c>
+      <c r="L5" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="M5" s="9">
+        <f>K5+L5</f>
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="N5" s="26">
+        <f>M5+(N3-M3)</f>
+        <v>0.8125</v>
+      </c>
+      <c r="O5" s="19"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="30"/>
+      <c r="T5" s="19"/>
+    </row>
+    <row r="6" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="22">
+        <v>2</v>
+      </c>
+      <c r="D6" s="26">
+        <f>E6+(E5-D5)</f>
+        <v>0.97916666666666674</v>
+      </c>
+      <c r="E6" s="15">
+        <f>G6+F6</f>
+        <v>0.93750000000000011</v>
+      </c>
+      <c r="F6" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G6" s="14">
+        <f>H6+(H5-G5)</f>
+        <v>0.91666666666666674</v>
+      </c>
+      <c r="H6" s="15">
+        <f>J6+I6</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="I6" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="J6" s="14">
+        <f>K6+(K5-J5)</f>
+        <v>0.8125</v>
+      </c>
+      <c r="K6" s="9">
+        <f>M6+L6</f>
+        <v>0.78125000000000011</v>
+      </c>
+      <c r="L6" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="M6" s="13">
+        <f>N6+(N5-M5)</f>
+        <v>0.76041666666666674</v>
+      </c>
+      <c r="N6" s="12">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="O6" s="19"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="19"/>
+    </row>
+    <row r="7" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="22">
+        <v>1</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0.75</v>
+      </c>
+      <c r="E7" s="16">
+        <f>D7+(E5-D5)</f>
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F7" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G7" s="10">
+        <f>E7+F7</f>
+        <v>0.8125</v>
+      </c>
+      <c r="H7" s="16">
+        <f>G7+(H5-G5)</f>
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="I7" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="J7" s="10">
+        <f>H7+I7</f>
+        <v>0.91666666666666674</v>
+      </c>
+      <c r="K7" s="16">
+        <f>J7+(K5-J5)</f>
+        <v>0.94791666666666663</v>
+      </c>
+      <c r="L7" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="M7" s="9">
+        <f>K7+L7</f>
+        <v>0.96875</v>
+      </c>
+      <c r="N7" s="26">
+        <f>M7+(N5-M5)</f>
+        <v>1.0208333333333335</v>
+      </c>
+      <c r="O7" s="19"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="30"/>
+      <c r="T7" s="19"/>
+    </row>
+    <row r="8" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="22">
+        <v>2</v>
+      </c>
+      <c r="D8" s="26">
+        <f>E8+(E7-D7)</f>
+        <v>1.1458333333333335</v>
+      </c>
+      <c r="E8" s="15">
+        <f>G8+F8</f>
+        <v>1.1041666666666667</v>
+      </c>
+      <c r="F8" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G8" s="14">
+        <f>H8+(H7-G7)</f>
+        <v>1.0833333333333335</v>
+      </c>
+      <c r="H8" s="15">
+        <f>J8+I8</f>
+        <v>1</v>
+      </c>
+      <c r="I8" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="J8" s="14">
+        <f>K8+(K7-J7)</f>
+        <v>0.97916666666666674</v>
+      </c>
+      <c r="K8" s="9">
+        <f>M8+L8</f>
+        <v>0.94791666666666685</v>
+      </c>
+      <c r="L8" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="M8" s="13">
+        <f>N8+(N7-M7)</f>
+        <v>0.92708333333333348</v>
+      </c>
+      <c r="N8" s="12">
+        <v>0.875</v>
+      </c>
+      <c r="O8" s="19"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="30"/>
+      <c r="T8" s="19"/>
+    </row>
+    <row r="9" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="22">
+        <v>1</v>
+      </c>
+      <c r="D9" s="12">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E9" s="16">
+        <f>D9+(E7-D7)</f>
+        <v>8.3333333333333287E-2</v>
+      </c>
+      <c r="F9" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G9" s="10">
+        <f>E9+F9</f>
+        <v>0.10416666666666662</v>
+      </c>
+      <c r="H9" s="16">
+        <f>G9+(H7-G7)</f>
+        <v>0.1875</v>
+      </c>
+      <c r="I9" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="J9" s="10">
+        <f>H9+I9</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="K9" s="16">
+        <f>J9+(K7-J7)</f>
+        <v>0.23958333333333323</v>
+      </c>
+      <c r="L9" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="M9" s="9">
+        <f>K9+L9</f>
+        <v>0.26041666666666657</v>
+      </c>
+      <c r="N9" s="26">
+        <f>M9+(N7-M7)</f>
+        <v>0.31250000000000006</v>
+      </c>
+      <c r="O9" s="19"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="30"/>
+      <c r="T9" s="19"/>
+    </row>
+    <row r="10" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="22">
+        <v>2</v>
+      </c>
+      <c r="D10" s="26">
+        <f>E10+(E9-D9)</f>
+        <v>0.89583333333333348</v>
+      </c>
+      <c r="E10" s="15">
+        <f>G10+F10</f>
+        <v>0.85416666666666685</v>
+      </c>
+      <c r="F10" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G10" s="14">
+        <f>H10+(H9-G9)</f>
+        <v>0.83333333333333348</v>
+      </c>
+      <c r="H10" s="15">
+        <f>J10+I10</f>
+        <v>0.75000000000000011</v>
+      </c>
+      <c r="I10" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="J10" s="14">
+        <f>K10+(K9-J9)</f>
+        <v>0.72916666666666674</v>
+      </c>
+      <c r="K10" s="9">
+        <f>M10+L10</f>
+        <v>0.69791666666666685</v>
+      </c>
+      <c r="L10" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="M10" s="13">
+        <f>N10+(N9-M9)</f>
+        <v>0.67708333333333348</v>
+      </c>
+      <c r="N10" s="12">
+        <v>0.625</v>
+      </c>
+      <c r="O10" s="19"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="30"/>
+      <c r="T10" s="19"/>
+    </row>
+    <row r="11" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="22">
+        <v>1</v>
+      </c>
+      <c r="D11" s="12">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E11" s="16">
+        <f>D11+(E9-D9)</f>
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="F11" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G11" s="10">
+        <f>E11+F11</f>
+        <v>0.52083333333333326</v>
+      </c>
+      <c r="H11" s="16">
+        <f>G11+(H9-G9)</f>
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="I11" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="J11" s="10">
+        <f>H11+I11</f>
+        <v>0.625</v>
+      </c>
+      <c r="K11" s="16">
+        <f>J11+(K9-J9)</f>
+        <v>0.65624999999999989</v>
+      </c>
+      <c r="L11" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="M11" s="9">
+        <f>K11+L11</f>
+        <v>0.67708333333333326</v>
+      </c>
+      <c r="N11" s="26">
+        <f>M11+(N9-M9)</f>
+        <v>0.72916666666666674</v>
+      </c>
+      <c r="O11" s="19"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="19"/>
+    </row>
+    <row r="12" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="22">
+        <v>2</v>
+      </c>
+      <c r="D12" s="26">
+        <f>E12+(E11-D11)</f>
+        <v>0.71875000000000022</v>
+      </c>
+      <c r="E12" s="15">
+        <f>G12+F12</f>
+        <v>0.67708333333333359</v>
+      </c>
+      <c r="F12" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G12" s="14">
+        <f>H12+(H11-G11)</f>
+        <v>0.65625000000000022</v>
+      </c>
+      <c r="H12" s="15">
+        <f>J12+I12</f>
+        <v>0.57291666666666685</v>
+      </c>
+      <c r="I12" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="J12" s="14">
+        <f>K12+(K11-J11)</f>
+        <v>0.55208333333333348</v>
+      </c>
+      <c r="K12" s="9">
+        <f>M12+L12</f>
+        <v>0.52083333333333359</v>
+      </c>
+      <c r="L12" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="M12" s="13">
+        <f>N12+(N11-M11)</f>
+        <v>0.50000000000000022</v>
+      </c>
+      <c r="N12" s="12">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="O12" s="19"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="30"/>
+      <c r="T12" s="19"/>
+    </row>
+    <row r="13" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="22">
+        <v>1</v>
+      </c>
+      <c r="D13" s="12">
+        <v>0.625</v>
+      </c>
+      <c r="E13" s="16">
+        <f>D13+(E11-D11)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F13" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G13" s="10">
+        <f>E13+F13</f>
+        <v>0.6875</v>
+      </c>
+      <c r="H13" s="16">
+        <f>G13+(H11-G11)</f>
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="I13" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="J13" s="10">
+        <f>H13+I13</f>
+        <v>0.79166666666666674</v>
+      </c>
+      <c r="K13" s="16">
+        <f>J13+(K11-J11)</f>
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="L13" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="M13" s="9">
+        <f>K13+L13</f>
+        <v>0.84375</v>
+      </c>
+      <c r="N13" s="26">
+        <f>M13+(N11-M11)</f>
+        <v>0.89583333333333348</v>
+      </c>
+      <c r="O13" s="19"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="19"/>
+    </row>
+    <row r="14" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="22">
+        <v>2</v>
+      </c>
+      <c r="D14" s="26">
+        <f>E14+(E13-D13)</f>
+        <v>0.81250000000000011</v>
+      </c>
+      <c r="E14" s="15">
+        <f>G14+F14</f>
+        <v>0.77083333333333348</v>
+      </c>
+      <c r="F14" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G14" s="14">
+        <f>H14+(H13-G13)</f>
+        <v>0.75000000000000011</v>
+      </c>
+      <c r="H14" s="15">
+        <f>J14+I14</f>
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="I14" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="J14" s="14">
+        <f>K14+(K13-J13)</f>
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="K14" s="9">
+        <f>M14+L14</f>
+        <v>0.61458333333333348</v>
+      </c>
+      <c r="L14" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="M14" s="13">
+        <f>N14+(N13-M13)</f>
+        <v>0.59375000000000011</v>
+      </c>
+      <c r="N14" s="12">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="O14" s="19"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="19"/>
+    </row>
+    <row r="15" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="22">
+        <v>1</v>
+      </c>
+      <c r="D15" s="12">
+        <v>0.875</v>
+      </c>
+      <c r="E15" s="16">
+        <f>D15+(E13-D13)</f>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F15" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G15" s="10">
+        <f>E15+F15</f>
+        <v>0.9375</v>
+      </c>
+      <c r="H15" s="16">
+        <f>G15+(H13-G13)</f>
+        <v>1.0208333333333335</v>
+      </c>
+      <c r="I15" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="J15" s="10">
+        <f>H15+I15</f>
+        <v>1.0416666666666667</v>
+      </c>
+      <c r="K15" s="16">
+        <f>J15+(K13-J13)</f>
+        <v>1.0729166666666665</v>
+      </c>
+      <c r="L15" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="M15" s="9">
+        <f>K15+L15</f>
+        <v>1.0937499999999998</v>
+      </c>
+      <c r="N15" s="26">
+        <f>M15+(N13-M13)</f>
+        <v>1.1458333333333333</v>
+      </c>
+      <c r="O15" s="19"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="30"/>
+      <c r="T15" s="19"/>
+    </row>
+    <row r="16" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="22">
+        <v>2</v>
+      </c>
+      <c r="D16" s="26">
+        <f>E16+(E15-D15)</f>
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E16" s="15">
+        <f>G16+F16</f>
+        <v>0.43750000000000006</v>
+      </c>
+      <c r="F16" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G16" s="14">
+        <f>H16+(H15-G15)</f>
+        <v>0.41666666666666674</v>
+      </c>
+      <c r="H16" s="15">
+        <f>J16+I16</f>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="I16" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="J16" s="14">
+        <f>K16+(K15-J15)</f>
+        <v>0.31249999999999994</v>
+      </c>
+      <c r="K16" s="9">
+        <f>M16+L16</f>
+        <v>0.28125000000000017</v>
+      </c>
+      <c r="L16" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="M16" s="13">
+        <f>N16+(N15-M15)</f>
+        <v>0.26041666666666685</v>
+      </c>
+      <c r="N16" s="12">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="O16" s="19"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="30"/>
+      <c r="T16" s="19"/>
+    </row>
+    <row r="17" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="22">
+        <v>1</v>
+      </c>
+      <c r="D17" s="12">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="E17" s="16">
+        <f>D17+(E15-D15)</f>
+        <v>0.24999999999999997</v>
+      </c>
+      <c r="F17" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G17" s="10">
+        <f>E17+F17</f>
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="H17" s="16">
+        <f>G17+(H15-G15)</f>
+        <v>0.3541666666666668</v>
+      </c>
+      <c r="I17" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="J17" s="10">
+        <f>H17+I17</f>
+        <v>0.37500000000000011</v>
+      </c>
+      <c r="K17" s="16">
+        <f>J17+(K15-J15)</f>
+        <v>0.40624999999999989</v>
+      </c>
+      <c r="L17" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="M17" s="9">
+        <f>K17+L17</f>
+        <v>0.4270833333333332</v>
+      </c>
+      <c r="N17" s="26">
+        <f>M17+(N15-M15)</f>
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="O17" s="19"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="30"/>
+      <c r="T17" s="19"/>
+    </row>
+    <row r="18" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="22">
+        <v>2</v>
+      </c>
+      <c r="D18" s="26">
+        <f>E18+(E17-D17)</f>
+        <v>1.2291666666666665</v>
+      </c>
+      <c r="E18" s="15">
+        <f>G18+F18</f>
+        <v>1.1875</v>
+      </c>
+      <c r="F18" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G18" s="14">
+        <f>H18+(H17-G17)</f>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="H18" s="15">
+        <f>J18+I18</f>
+        <v>1.0833333333333333</v>
+      </c>
+      <c r="I18" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="J18" s="14">
+        <f>K18+(K17-J17)</f>
+        <v>1.0625</v>
+      </c>
+      <c r="K18" s="9">
+        <f>M18+L18</f>
+        <v>1.0312500000000002</v>
+      </c>
+      <c r="L18" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="M18" s="13">
+        <f>N18+(N17-M17)</f>
+        <v>1.010416666666667</v>
+      </c>
+      <c r="N18" s="12">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="O18" s="19"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="30"/>
+      <c r="T18" s="19"/>
+    </row>
+    <row r="19" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="30"/>
+      <c r="T19" s="19"/>
+    </row>
+    <row r="20" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="22">
+      <c r="B20" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="22">
         <v>1</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="14">
+      <c r="D20" s="7"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="14">
         <v>0.5</v>
       </c>
-      <c r="K6" s="26"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="12">
+      <c r="N20" s="26"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="12">
         <v>0.375</v>
       </c>
-      <c r="N6" s="19"/>
-    </row>
-    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="T20" s="19"/>
+    </row>
+    <row r="21" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="22">
+      <c r="B21" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="22">
         <v>2</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="9">
+      <c r="D21" s="7"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="9">
         <v>0.625</v>
       </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="26">
+      <c r="N21" s="7"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="26">
         <v>0.75</v>
       </c>
-      <c r="N7" s="19"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="N8" s="25"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="25"/>
-      <c r="N9" s="25"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="N10" s="25"/>
-    </row>
-    <row r="1048544" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1048544" s="18"/>
+      <c r="T21" s="19"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="22">
+        <v>1</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="14">
+        <v>0</v>
+      </c>
+      <c r="N22" s="26"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="19"/>
+      <c r="S22" s="12">
+        <v>0.875</v>
+      </c>
+      <c r="T22" s="25"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="22">
+        <v>2</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="9">
+        <v>0.125</v>
+      </c>
+      <c r="N23" s="7"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="26"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="19"/>
+      <c r="S23" s="26">
+        <v>0.25</v>
+      </c>
+      <c r="T23" s="25"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="22">
+        <v>1</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="N24" s="7"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="26"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="T24" s="25"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="22">
+        <v>2</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="N25" s="7"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="26"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="26">
+        <v>0.375</v>
+      </c>
+      <c r="T25" s="25"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="22">
+        <v>1</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="14">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="N26" s="7"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="12">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="T26" s="25"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="22">
+        <v>2</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="9">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="N27" s="7"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="26"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="26">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="T27" s="25"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="22">
+        <v>1</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="14">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="N28" s="7"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="26"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="12">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="T28" s="25"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="22">
+        <v>2</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="9">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="N29" s="7"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="26"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="26">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="T29" s="25"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="22">
+        <v>1</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="14">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="N30" s="7"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="26"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="12">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="T30" s="25"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="22">
+        <v>2</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="9">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="N31" s="7"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="26"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="26">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="T31" s="25"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="22">
+        <v>1</v>
+      </c>
+      <c r="J33" s="10">
+        <v>0.375</v>
+      </c>
+      <c r="O33" s="27"/>
+      <c r="P33" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="22">
+        <v>2</v>
+      </c>
+      <c r="J34" s="14">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="P34" s="12">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="22">
+        <v>1</v>
+      </c>
+      <c r="J35" s="10">
+        <v>0.875</v>
+      </c>
+      <c r="P35" s="26">
+        <v>0.91666666666666663</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="22">
+        <v>2</v>
+      </c>
+      <c r="J36" s="14">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="P36" s="12">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="22">
+        <v>1</v>
+      </c>
+      <c r="J37" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="O37" s="44"/>
+      <c r="P37" s="14">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="22">
+        <v>2</v>
+      </c>
+      <c r="J38" s="14">
+        <v>0.375</v>
+      </c>
+      <c r="P38" s="12">
+        <v>0.29166666666666669</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="22">
+        <v>1</v>
+      </c>
+      <c r="J39" s="10">
+        <v>0.625</v>
+      </c>
+      <c r="P39" s="26">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="22">
+        <v>2</v>
+      </c>
+      <c r="J40" s="14">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="P40" s="12">
+        <v>0.45833333333333331</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" s="22">
+        <v>1</v>
+      </c>
+      <c r="J41" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="O41" s="44"/>
+      <c r="P41" s="14">
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="22">
+        <v>2</v>
+      </c>
+      <c r="J42" s="14">
+        <v>0.8125</v>
+      </c>
+      <c r="P42" s="12">
+        <v>0.72916666666666663</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" s="22">
+        <v>1</v>
+      </c>
+      <c r="J43" s="10">
+        <v>0.125</v>
+      </c>
+      <c r="P43" s="26">
+        <v>0.20833333333333334</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="22">
+        <v>2</v>
+      </c>
+      <c r="J44" s="14">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="P44" s="12">
+        <v>0.89583333333333337</v>
+      </c>
+    </row>
+    <row r="1048567" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1048567" s="18"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:K7" xr:uid="{A2F39999-98DD-4F29-9CE9-B5711A0A92DD}"/>
-  <mergeCells count="2">
+  <mergeCells count="3">
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
     <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="43" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>